<commit_message>
[Pipette] F/W 작업분 update
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/3_Firmware/Plasma Pipette FW Issue list.xlsx
+++ b/1_Plasma_Pipette/3_Firmware/Plasma Pipette FW Issue list.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CC618A-6FB4-4184-81ED-09CC1493E678}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issue list" sheetId="1" r:id="rId1"/>
@@ -12,12 +13,15 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Issue list'!$A$4:$G$4</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -380,11 +384,49 @@
 RCC_ClkInitStruct.APB1CLKDivider = RCC_HCLK_DIV1;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Power Off가 안됨.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEY_PWR_Pin GPIO 설정 변경
+NOPULL -&gt; PULLDOWN (Gpio.c)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On Key 동작 안됨.
+ Default Low 유지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충전중 Plasma 동작 안하도록 수정하며 생긴 문제임
+USB_DET_Pin GPIO 설정 변경
+NOPULL -&gt; PULLDOWN (Gpio.c)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPEN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완충 인식 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On후 5초후 S/V On 지원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_state.c - Line 24 수정
+                GPIO_ENABLE(GAS_EN);
+                vTaskDelay( 5000); // 2019.01.17 Arvid - Plasma On delay 5sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,7 +452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,8 +471,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -618,11 +666,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -649,9 +723,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -741,6 +812,45 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -782,6 +892,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -804,7 +917,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1"/>
+        <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -878,7 +997,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2"/>
+        <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -965,7 +1090,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+        <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1077,7 +1208,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5"/>
+        <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1151,7 +1288,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6"/>
+        <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1221,7 +1364,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7"/>
+        <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1291,7 +1440,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+        <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1413,18 +1568,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
               <a:solidFill>
@@ -1492,18 +1635,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
               <a:solidFill>
@@ -1571,18 +1702,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
               <a:solidFill>
@@ -1752,7 +1871,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9"/>
+        <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1822,7 +1947,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
+        <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1892,7 +2023,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11"/>
+        <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1962,7 +2099,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="모서리가 둥근 직사각형 13"/>
+        <xdr:cNvPr id="14" name="모서리가 둥근 직사각형 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2032,7 +2175,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="모서리가 둥근 직사각형 14"/>
+        <xdr:cNvPr id="15" name="모서리가 둥근 직사각형 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2100,18 +2249,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
               <a:solidFill>
@@ -2475,18 +2612,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
               <a:solidFill>
@@ -2593,18 +2718,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
               <a:solidFill>
@@ -2658,18 +2771,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0">
               <a:solidFill>
@@ -2755,7 +2856,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="모서리가 둥근 직사각형 15"/>
+        <xdr:cNvPr id="16" name="모서리가 둥근 직사각형 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2829,7 +2936,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="모서리가 둥근 직사각형 16"/>
+        <xdr:cNvPr id="17" name="모서리가 둥근 직사각형 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2899,7 +3012,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 17"/>
+        <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2969,7 +3088,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="모서리가 둥근 직사각형 18"/>
+        <xdr:cNvPr id="19" name="모서리가 둥근 직사각형 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3039,7 +3164,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="모서리가 둥근 직사각형 19"/>
+        <xdr:cNvPr id="20" name="모서리가 둥근 직사각형 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3109,7 +3240,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="모서리가 둥근 직사각형 20"/>
+        <xdr:cNvPr id="21" name="모서리가 둥근 직사각형 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3179,7 +3316,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="모서리가 둥근 직사각형 21"/>
+        <xdr:cNvPr id="22" name="모서리가 둥근 직사각형 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3280,7 +3423,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3313,9 +3456,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3348,6 +3508,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3523,54 +3700,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="4.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="77.09765625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:7" s="5" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="31" t="s">
+    <row r="3" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:7" s="5" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="15">
+    <row r="5" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B5" s="14">
         <v>1</v>
       </c>
       <c r="C5" s="6">
         <v>43246</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="36" t="s">
         <v>80</v>
       </c>
       <c r="E5" s="6">
@@ -3579,36 +3756,36 @@
       <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="39">
+    <row r="6" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B6" s="38">
         <v>2</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="39">
         <v>43246</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="42" t="s">
+      <c r="E6" s="39"/>
+      <c r="F6" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="42" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="16">
+    <row r="7" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B7" s="15">
         <v>3</v>
       </c>
       <c r="C7" s="8">
         <v>43246</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="37" t="s">
         <v>80</v>
       </c>
       <c r="E7" s="8">
@@ -3617,18 +3794,18 @@
       <c r="F7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="16">
+    <row r="8" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B8" s="15">
         <v>4</v>
       </c>
       <c r="C8" s="8">
         <v>43246</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="37" t="s">
         <v>80</v>
       </c>
       <c r="E8" s="8">
@@ -3637,38 +3814,38 @@
       <c r="F8" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="66" x14ac:dyDescent="0.3">
-      <c r="B9" s="16">
+    <row r="9" spans="2:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="B9" s="15">
         <v>5</v>
       </c>
       <c r="C9" s="8">
         <v>43246</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="37" t="s">
         <v>80</v>
       </c>
       <c r="E9" s="8">
         <v>43258</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="B10" s="16">
+    <row r="10" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B10" s="15">
         <v>6</v>
       </c>
       <c r="C10" s="8">
         <v>43246</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>80</v>
       </c>
       <c r="E10" s="8">
@@ -3677,38 +3854,38 @@
       <c r="F10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="66" x14ac:dyDescent="0.3">
-      <c r="B11" s="16">
+    <row r="11" spans="2:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="B11" s="15">
         <v>7</v>
       </c>
       <c r="C11" s="8">
         <v>43246</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="37" t="s">
         <v>80</v>
       </c>
       <c r="E11" s="8">
         <v>43256</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="16">
+    <row r="12" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B12" s="15">
         <v>8</v>
       </c>
       <c r="C12" s="8">
         <v>43246</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="37" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="8">
@@ -3717,18 +3894,18 @@
       <c r="F12" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="B13" s="16">
+    <row r="13" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B13" s="15">
         <v>9</v>
       </c>
       <c r="C13" s="8">
         <v>43258</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>80</v>
       </c>
       <c r="E13" s="8">
@@ -3737,59 +3914,152 @@
       <c r="F13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="16">
+    <row r="14" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B14" s="15">
         <v>10</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="46">
+        <v>43458</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>80</v>
+      </c>
       <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16">
+      <c r="F14" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B15" s="15">
         <v>11</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="46">
+        <v>43459</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="43"/>
+      <c r="F15" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B16" s="15">
+        <v>12</v>
+      </c>
+      <c r="C16" s="8">
+        <v>43466</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="43"/>
+      <c r="F16" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="45"/>
+    </row>
+    <row r="17" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B17" s="15">
+        <v>13</v>
+      </c>
+      <c r="C17" s="8">
+        <v>43481</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="43">
+        <v>43482</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B18" s="15">
+        <v>14</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B19" s="15">
+        <v>15</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B20" s="15">
+        <v>16</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
+    </row>
+    <row r="21" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="15">
+        <v>17</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="54"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C23" s="2"/>
+      <c r="D23" s="54"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C24" s="2"/>
+      <c r="D24" s="54"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C25" s="2"/>
+      <c r="D25" s="54"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C26" s="2"/>
+      <c r="D26" s="54"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C27" s="2"/>
+      <c r="D27" s="54"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C28" s="2"/>
+      <c r="D28" s="54"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:G4" xr:uid="{156A324A-EEBF-442D-8ABE-045039FBF5BD}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -3797,347 +4067,347 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.125" customWidth="1"/>
+    <col min="4" max="4" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.09765625" customWidth="1"/>
     <col min="6" max="6" width="9" style="3"/>
-    <col min="7" max="7" width="52.875" customWidth="1"/>
+    <col min="7" max="7" width="52.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:7" s="17" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="47" t="s">
+    <row r="2" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="2:7" s="16" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="26" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="49" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B4" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="50"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="20" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B5" s="62"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="50"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="20" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B6" s="62"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="50"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="20" t="s">
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B7" s="62"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="50" t="s">
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B8" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="56" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="50"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="20" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B9" s="62"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="44"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="50"/>
-      <c r="C10" s="46" t="s">
+      <c r="G9" s="56"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B10" s="62"/>
+      <c r="C10" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="50"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="20" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B11" s="62"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="44"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="50"/>
-      <c r="C12" s="46" t="s">
+      <c r="G11" s="56"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B12" s="62"/>
+      <c r="C12" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="50"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="20" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B13" s="62"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="44"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="50"/>
-      <c r="C14" s="22" t="s">
+      <c r="G13" s="56"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B14" s="62"/>
+      <c r="C14" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="34" t="s">
+      <c r="E14" s="64"/>
+      <c r="F14" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="50" t="s">
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B15" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="50"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="20" t="s">
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B16" s="62"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="21"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="50"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="20" t="s">
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B17" s="62"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="50"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="20" t="s">
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B18" s="62"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="21"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="50"/>
-      <c r="C19" s="46" t="s">
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B19" s="62"/>
+      <c r="C19" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="50"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="20" t="s">
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B20" s="62"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="21"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="50"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="20" t="s">
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B21" s="62"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="21"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="50"/>
-      <c r="C22" s="23" t="s">
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B22" s="62"/>
+      <c r="C22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="21"/>
-    </row>
-    <row r="23" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="53"/>
-      <c r="C23" s="24" t="s">
+      <c r="E22" s="64"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="65"/>
+      <c r="C23" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="34" t="s">
+      <c r="E23" s="63"/>
+      <c r="F23" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="25"/>
+      <c r="G23" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -4164,30 +4434,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B4:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.375" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="27.75" customWidth="1"/>
-    <col min="7" max="7" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.3984375" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" customWidth="1"/>
+    <col min="4" max="4" width="27.69921875" customWidth="1"/>
+    <col min="7" max="7" width="32.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="46" t="s">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B4" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>66</v>
       </c>
       <c r="G4" t="s">
@@ -4200,12 +4470,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="46"/>
-      <c r="C5" s="20" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B5" s="58"/>
+      <c r="C5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>49</v>
       </c>
       <c r="G5" t="s">
@@ -4218,16 +4488,16 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="46"/>
-      <c r="C6" s="20" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B6" s="58"/>
+      <c r="C6" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="G7" t="s">
         <v>63</v>
       </c>
@@ -4235,7 +4505,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="G8">
         <v>0</v>
       </c>
@@ -4244,7 +4514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="G9">
         <v>1</v>
       </c>
@@ -4253,7 +4523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="G10">
         <v>2</v>
       </c>
@@ -4273,14 +4543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>